<commit_message>
update corona report (mit boostern)
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2021-09-12.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2021-09-12.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="342">
   <si>
     <t xml:space="preserve">Geimpfte Personen</t>
   </si>
@@ -30,7 +30,7 @@
     <t xml:space="preserve">Vorwoche</t>
   </si>
   <si>
-    <t xml:space="preserve">Stand 13.9.</t>
+    <t xml:space="preserve">Stand 17.9.</t>
   </si>
   <si>
     <t xml:space="preserve">Anteil_Veraenderung</t>
@@ -45,10 +45,10 @@
     <t xml:space="preserve">Gesamt</t>
   </si>
   <si>
-    <t xml:space="preserve">54721636 (65,8 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55315227 (66,5 %)</t>
+    <t xml:space="preserve">55144235 (66,3 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55703730 (67,0 %)</t>
   </si>
   <si>
     <t xml:space="preserve"> 0,7 PP</t>
@@ -57,22 +57,22 @@
     <t xml:space="preserve">Nicht vollst. geimpft</t>
   </si>
   <si>
-    <t xml:space="preserve">3727971 ( 4,5 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3604954 ( 4,3 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0,1 PP</t>
+    <t xml:space="preserve">3678993 ( 4,4 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3459229 ( 4,2 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0,3 PP</t>
   </si>
   <si>
     <t xml:space="preserve">Vollst. geimpft</t>
   </si>
   <si>
-    <t xml:space="preserve">50993665 (61,3 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">51710273 (62,2 %)</t>
+    <t xml:space="preserve">51465242 (61,9 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52244501 (62,8 %)</t>
   </si>
   <si>
     <t xml:space="preserve"> 0,9 PP</t>
@@ -81,10 +81,13 @@
     <t xml:space="preserve">Zusätzl. Booster-Impfung</t>
   </si>
   <si>
-    <t xml:space="preserve">194108 ( 0,2 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  NA PP</t>
+    <t xml:space="preserve">162467 ( 0,2 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">328459 ( 0,4 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0,2 PP</t>
   </si>
   <si>
     <t xml:space="preserve">Impffortschritt</t>
@@ -102,40 +105,40 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">   NA %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1641741</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1382991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-15,8 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">davon in Impfzentren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">943832 ( 57,5 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">725299 ( 52,4 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-23,2 %</t>
+    <t xml:space="preserve">  NA %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1398188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1285990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-8,0 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">davon in Impfzentren und Betrieben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">740496 ( 53 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667112 ( 51,9 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-9,9 %</t>
   </si>
   <si>
     <t xml:space="preserve">davon in ärztl. Praxen</t>
   </si>
   <si>
-    <t xml:space="preserve">697909 ( 42,5 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">657692 ( 47,6 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -5,8 %</t>
+    <t xml:space="preserve">657692 ( 47 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">618878 ( 48,1 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5,9 %</t>
   </si>
   <si>
     <t xml:space="preserve">Bundesland</t>
@@ -159,160 +162,166 @@
     <t xml:space="preserve">7-Tage-Inzidenz 60+</t>
   </si>
   <si>
+    <t xml:space="preserve">67,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baden-Württemberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bayern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berlin</t>
+  </si>
+  <si>
     <t xml:space="preserve">66,5</t>
   </si>
   <si>
-    <t xml:space="preserve">62,2</t>
+    <t xml:space="preserve">62,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brandenburg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57,1</t>
   </si>
   <si>
     <t xml:space="preserve">0,2</t>
   </si>
   <si>
-    <t xml:space="preserve">Baden-Württemberg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">63,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bayern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">63,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Berlin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66,1</t>
+    <t xml:space="preserve">Bremen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hamburg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hessen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66,8</t>
   </si>
   <si>
     <t xml:space="preserve">62,1</t>
   </si>
   <si>
-    <t xml:space="preserve">Brandenburg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56,5</t>
+    <t xml:space="preserve">Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niedersachsen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69,8</t>
   </si>
   <si>
     <t xml:space="preserve">0,1</t>
   </si>
   <si>
-    <t xml:space="preserve">Bremen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hamburg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hessen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mecklenburg-Vorpommern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Niedersachsen</t>
+    <t xml:space="preserve">Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saarland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73,0</t>
   </si>
   <si>
     <t xml:space="preserve">69,3</t>
   </si>
   <si>
-    <t xml:space="preserve">64,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nordrhein-Westfalen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rheinland-Pfalz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saarland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68,7</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sachsen</t>
   </si>
   <si>
-    <t xml:space="preserve">56,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">52,9</t>
+    <t xml:space="preserve">56,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53,4</t>
   </si>
   <si>
     <t xml:space="preserve">Sachsen-Anhalt</t>
   </si>
   <si>
-    <t xml:space="preserve">58,8</t>
+    <t xml:space="preserve">62,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59,3</t>
   </si>
   <si>
     <t xml:space="preserve">Schleswig-Holstein</t>
   </si>
   <si>
-    <t xml:space="preserve">71,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,5</t>
+    <t xml:space="preserve">71,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67,5</t>
   </si>
   <si>
     <t xml:space="preserve">Thüringen</t>
   </si>
   <si>
-    <t xml:space="preserve">59,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56,8</t>
+    <t xml:space="preserve">59,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57,2</t>
   </si>
   <si>
     <t xml:space="preserve">Impfstoffdosen</t>
@@ -324,28 +333,28 @@
     <t xml:space="preserve">Biontech/Pfizer</t>
   </si>
   <si>
-    <t xml:space="preserve">77792582 (47,4 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79045361 (47,8 %)</t>
+    <t xml:space="preserve">78692493 (47,4 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79939562 (47,7 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Erstimpfungen</t>
   </si>
   <si>
-    <t xml:space="preserve">38185387</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38672744</t>
+    <t xml:space="preserve">38539475</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38991699</t>
   </si>
   <si>
     <t xml:space="preserve">Zweitimpfungen</t>
   </si>
   <si>
-    <t xml:space="preserve">39607195</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40190740</t>
+    <t xml:space="preserve">40000635</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40635870</t>
   </si>
   <si>
     <t xml:space="preserve">Booster</t>
@@ -354,37 +363,40 @@
     <t xml:space="preserve">0</t>
   </si>
   <si>
-    <t xml:space="preserve">181877</t>
+    <t xml:space="preserve">311993</t>
   </si>
   <si>
     <t xml:space="preserve">geliefert</t>
   </si>
   <si>
-    <t xml:space="preserve">82900542</t>
+    <t xml:space="preserve">83717136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84062286</t>
   </si>
   <si>
     <t xml:space="preserve">Moderna</t>
   </si>
   <si>
-    <t xml:space="preserve">9447848 ( 5,8 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9523981 ( 5,8 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4408814</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4425806</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5039034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5086530</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11645</t>
+    <t xml:space="preserve">9496283 ( 5,7 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9564338 ( 5,7 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4420627</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4435406</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5066122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5113113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15819</t>
   </si>
   <si>
     <t xml:space="preserve">12836080</t>
@@ -393,117 +405,123 @@
     <t xml:space="preserve">AstraZeneca</t>
   </si>
   <si>
-    <t xml:space="preserve">12652767 ( 7,7 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12671108 ( 7,7 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9216383</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9227365</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3436384</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3443691</t>
-  </si>
-  <si>
-    <t xml:space="preserve">52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14413830</t>
+    <t xml:space="preserve">12667902 ( 7,6 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12678096 ( 7,6 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9226749</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9229571</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3441101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3448464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14420360</t>
   </si>
   <si>
     <t xml:space="preserve">Johnson&amp;Johnson</t>
   </si>
   <si>
-    <t xml:space="preserve">2911052 ( 1,8 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2989846 ( 1,8 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">534</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4237395</t>
+    <t xml:space="preserve">2957882 ( 1,8 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3047640 ( 1,8 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einzeldosisimpfung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2957384</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3047054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">586</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4370545</t>
   </si>
   <si>
     <t xml:space="preserve">Testungen</t>
   </si>
   <si>
-    <t xml:space="preserve">KW 35</t>
+    <t xml:space="preserve">KW 36</t>
   </si>
   <si>
     <t xml:space="preserve">Zahl der PCR-Tests</t>
   </si>
   <si>
-    <t xml:space="preserve">748019</t>
-  </si>
-  <si>
     <t xml:space="preserve">833546</t>
   </si>
   <si>
-    <t xml:space="preserve">11 %</t>
+    <t xml:space="preserve">882536</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 %</t>
   </si>
   <si>
     <t xml:space="preserve">Positive Tests</t>
   </si>
   <si>
-    <t xml:space="preserve">64670</t>
-  </si>
-  <si>
     <t xml:space="preserve">75930</t>
   </si>
   <si>
-    <t xml:space="preserve">17,4 %</t>
+    <t xml:space="preserve">74023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2,5 %</t>
   </si>
   <si>
     <t xml:space="preserve">Positivrate</t>
   </si>
   <si>
-    <t xml:space="preserve">8,65 %</t>
-  </si>
-  <si>
     <t xml:space="preserve">9,11 %</t>
   </si>
   <si>
-    <t xml:space="preserve">0,46 PP</t>
+    <t xml:space="preserve">8,39 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0,72 PP</t>
   </si>
   <si>
     <t xml:space="preserve">Testkapazität</t>
   </si>
   <si>
-    <t xml:space="preserve">1906542</t>
-  </si>
-  <si>
     <t xml:space="preserve">1972098</t>
   </si>
   <si>
-    <t xml:space="preserve">3 %</t>
+    <t xml:space="preserve">1976742</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 %</t>
   </si>
   <si>
     <t xml:space="preserve">Auslastung</t>
   </si>
   <si>
-    <t xml:space="preserve">39 %</t>
-  </si>
-  <si>
     <t xml:space="preserve">42 %</t>
   </si>
   <si>
+    <t xml:space="preserve">45 %</t>
+  </si>
+  <si>
     <t xml:space="preserve">3 PP</t>
   </si>
   <si>
     <t xml:space="preserve">R-Wert &amp; 7-Tage-Inzidenz</t>
   </si>
   <si>
-    <t xml:space="preserve">KW 36</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reproduktionszahl R</t>
   </si>
   <si>
@@ -513,7 +531,7 @@
     <t xml:space="preserve">1,04</t>
   </si>
   <si>
-    <t xml:space="preserve"> -8,8 %</t>
+    <t xml:space="preserve">-8,8 %</t>
   </si>
   <si>
     <t xml:space="preserve">Neue Fälle je 100.000 EW in 7 Tagen bezogen auf die jeweilige Gruppe:</t>
@@ -522,10 +540,10 @@
     <t xml:space="preserve">90</t>
   </si>
   <si>
-    <t xml:space="preserve">87</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -3,3 %</t>
+    <t xml:space="preserve">86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4,4 %</t>
   </si>
   <si>
     <t xml:space="preserve">- Davon Unter-14-Jährige</t>
@@ -534,10 +552,10 @@
     <t xml:space="preserve">165</t>
   </si>
   <si>
-    <t xml:space="preserve">150</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -9,1 %</t>
+    <t xml:space="preserve">156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5,5 %</t>
   </si>
   <si>
     <t xml:space="preserve">- Davon 15-bis-34-Jährige</t>
@@ -546,10 +564,10 @@
     <t xml:space="preserve">144</t>
   </si>
   <si>
-    <t xml:space="preserve">126</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-12,5 %</t>
+    <t xml:space="preserve">132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-8,3 %</t>
   </si>
   <si>
     <t xml:space="preserve">- Davon 35-bis-59-Jährige</t>
@@ -558,10 +576,7 @@
     <t xml:space="preserve">79</t>
   </si>
   <si>
-    <t xml:space="preserve">73</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -7,6 %</t>
+    <t xml:space="preserve">77</t>
   </si>
   <si>
     <t xml:space="preserve">- Davon 60-bis-79-Jährige</t>
@@ -570,7 +585,10 @@
     <t xml:space="preserve">23</t>
   </si>
   <si>
-    <t xml:space="preserve">  0,0 %</t>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4,3 %</t>
   </si>
   <si>
     <t xml:space="preserve">- Davon Über-80-Jährige</t>
@@ -579,97 +597,97 @@
     <t xml:space="preserve">26</t>
   </si>
   <si>
-    <t xml:space="preserve">28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  7,7 %</t>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15,4 %</t>
   </si>
   <si>
     <t xml:space="preserve">Hospitalisierungen</t>
   </si>
   <si>
-    <t xml:space="preserve">KW 33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1512 ( 4,7%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2062 ( 4,2%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36,4 %</t>
+    <t xml:space="preserve">KW 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2128 ( 4,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2795 ( 4,2%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31,3 %</t>
   </si>
   <si>
     <t xml:space="preserve">Davon unter 4-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">55 ( 4,5%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70 ( 3,8%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27,3 %</t>
+    <t xml:space="preserve">73 ( 3,9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82 ( 2,8%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,3 %</t>
   </si>
   <si>
     <t xml:space="preserve">Davon 5- bis 14-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">35 ( 0,8%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53 ( 0,6%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">51,4 %</t>
+    <t xml:space="preserve">54 ( 0,6%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63 ( 0,5%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16,7 %</t>
   </si>
   <si>
     <t xml:space="preserve">Davon 15- bis 34-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">346 ( 2,4%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">470 ( 2,3%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35,8 %</t>
+    <t xml:space="preserve">486 ( 2,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">577 ( 2,2%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18,7 %</t>
   </si>
   <si>
     <t xml:space="preserve">Davon 35- bis 59-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">604 ( 6,3%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">854 ( 5,7%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41,4 %</t>
+    <t xml:space="preserve">880 ( 5,9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1186 ( 5,8%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34,8 %</t>
   </si>
   <si>
     <t xml:space="preserve">Davon 60- bis 79-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">308 (18,8%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400 (17,8%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29,9 %</t>
+    <t xml:space="preserve">412 (18,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">558 (16,8%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35,4 %</t>
   </si>
   <si>
     <t xml:space="preserve">Davon über 80-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">164 (32,3%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">215 (32,9%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31,1 %</t>
+    <t xml:space="preserve">223 (34,0%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">329 (31,8%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47,5 %</t>
   </si>
   <si>
     <t xml:space="preserve">Intensivbetten</t>
@@ -715,91 +733,91 @@
     <t xml:space="preserve">Todesfälle &amp; Sterblichkeit</t>
   </si>
   <si>
-    <t xml:space="preserve">KW 31</t>
+    <t xml:space="preserve">KW 32</t>
   </si>
   <si>
     <t xml:space="preserve">0 bis 59 Jahre</t>
   </si>
   <si>
-    <t xml:space="preserve">14 ( 0,1%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 ( 0,0%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-57,1%</t>
+    <t xml:space="preserve">8 ( 0,0%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 ( 0,1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200,0%</t>
   </si>
   <si>
     <t xml:space="preserve">60 bis 79 Jahre</t>
   </si>
   <si>
-    <t xml:space="preserve">24 ( 2,7%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 ( 2,2%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -4,2%</t>
+    <t xml:space="preserve">24 ( 2,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43 ( 2,6%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 79,2%</t>
   </si>
   <si>
     <t xml:space="preserve">80 Jahre +</t>
   </si>
   <si>
-    <t xml:space="preserve">24 (10,3%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40 (12,3%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 66,7%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62 ( 0,4%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69 ( 0,3%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 11,3%</t>
+    <t xml:space="preserve">42 (12,9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53 (10,5%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 26,2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74 ( 0,4%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120 ( 0,4%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 62,2%</t>
   </si>
   <si>
     <t xml:space="preserve">Übersterblichkeit</t>
   </si>
   <si>
-    <t xml:space="preserve">-160 (-9,4%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-112 (-6,5%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 30,0%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-465 (-7,6%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-468 (-7,8%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -0,6%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">92 ( 0,9%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">142 ( 1,5%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 54,3%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-533 (-3,0%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-438 (-2,5%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 17,8%</t>
+    <t xml:space="preserve">-122 (-7,1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-50 (-3,1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 59,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-502 (-8,4%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-256 (-4,4%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 49,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">114 ( 1,2%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1138 (12,6%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">898,2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-510 (-2,9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">832 ( 5,0%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">263,1%</t>
   </si>
   <si>
     <t xml:space="preserve">Bereits infizierte Bevölkerung</t>
@@ -826,7 +844,7 @@
     <t xml:space="preserve">5,3 %</t>
   </si>
   <si>
-    <t xml:space="preserve">1,08</t>
+    <t xml:space="preserve">1,09</t>
   </si>
   <si>
     <t xml:space="preserve">5,4 %</t>
@@ -874,7 +892,7 @@
     <t xml:space="preserve">0,93</t>
   </si>
   <si>
-    <t xml:space="preserve">15.09.2021</t>
+    <t xml:space="preserve">18.09.2021</t>
   </si>
   <si>
     <t xml:space="preserve">4,2 %</t>
@@ -892,7 +910,7 @@
     <t xml:space="preserve">7,2 %</t>
   </si>
   <si>
-    <t xml:space="preserve">1,35</t>
+    <t xml:space="preserve">1,37</t>
   </si>
   <si>
     <t xml:space="preserve">4,6 %</t>
@@ -910,7 +928,7 @@
     <t xml:space="preserve">6,2 %</t>
   </si>
   <si>
-    <t xml:space="preserve">1,38</t>
+    <t xml:space="preserve">1,40</t>
   </si>
   <si>
     <t xml:space="preserve">Fälle gesamt</t>
@@ -976,52 +994,49 @@
     <t xml:space="preserve">2,6 %</t>
   </si>
   <si>
+    <t xml:space="preserve">Frankreich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,3 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deutschland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,3 %</t>
+  </si>
+  <si>
     <t xml:space="preserve">Belgien</t>
   </si>
   <si>
-    <t xml:space="preserve">2,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schweden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11,3 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deutschland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,3 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frankreich</t>
-  </si>
-  <si>
     <t xml:space="preserve">2,3</t>
   </si>
   <si>
+    <t xml:space="preserve">10,8 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,1 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,4</t>
+  </si>
+  <si>
     <t xml:space="preserve">10,7 %</t>
   </si>
   <si>
-    <t xml:space="preserve">2,1 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,3</t>
-  </si>
-  <si>
     <t xml:space="preserve">1,9 %</t>
   </si>
   <si>
-    <t xml:space="preserve">0,8</t>
-  </si>
-  <si>
     <t xml:space="preserve">10,5 %</t>
   </si>
   <si>
     <t xml:space="preserve">1,8 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,6</t>
   </si>
   <si>
     <t xml:space="preserve">10,4 %</t>
@@ -1438,12 +1453,14 @@
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6"/>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1462,25 +1479,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C1" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D1" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
       <c r="G1" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2">
@@ -1488,128 +1505,128 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="C2" t="n">
         <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="E2" t="n">
         <v>26</v>
       </c>
       <c r="F2" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="C3" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="E3" t="n">
         <v>31</v>
       </c>
       <c r="F3" t="n">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G3" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="C4" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="E4" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F4" t="n">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="G4" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="C5" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="E5" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" t="n">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" t="n">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>276</v>
+      </c>
+      <c r="E6" t="n">
+        <v>12</v>
+      </c>
+      <c r="F6" t="n">
+        <v>46</v>
+      </c>
+      <c r="G6" t="s">
         <v>269</v>
-      </c>
-      <c r="C6" t="n">
-        <v>70</v>
-      </c>
-      <c r="D6" t="s">
-        <v>270</v>
-      </c>
-      <c r="E6" t="n">
-        <v>13</v>
-      </c>
-      <c r="F6" t="n">
-        <v>49</v>
-      </c>
-      <c r="G6" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="C7" t="n">
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="E7" t="n">
         <v>21</v>
@@ -1618,260 +1635,260 @@
         <v>117</v>
       </c>
       <c r="G7" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="C8" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="E8" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F8" t="n">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G8" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="C9" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="E9" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" t="n">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G9" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="C10" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="E10" t="n">
         <v>10</v>
       </c>
       <c r="F10" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="C11" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="E11" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" t="n">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G11" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B12" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C12" t="n">
         <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="E12" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F12" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G12" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="C13" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="E13" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G13" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="C14" t="n">
         <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="E14" t="n">
         <v>23</v>
       </c>
       <c r="F14" t="n">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G14" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="C15" t="n">
         <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="E15" t="n">
         <v>17</v>
       </c>
       <c r="F15" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G15" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B16" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="C16" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="E16" t="n">
         <v>11</v>
       </c>
       <c r="F16" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="C17" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="E17" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G17" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="C18" t="n">
         <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="E18" t="n">
         <v>18</v>
       </c>
       <c r="F18" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G18" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -1890,121 +1907,121 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="B1" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="C1" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="D1" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="E1" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="F1" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="G1" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="H1" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="I1" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="J1" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="B2" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="C2" t="n">
-        <v>1682926</v>
+        <v>1683179</v>
       </c>
       <c r="D2" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="E2" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="F2" t="n">
-        <v>129885</v>
+        <v>129919</v>
       </c>
       <c r="G2" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="H2" t="n">
-        <v>693</v>
+        <v>736</v>
       </c>
       <c r="I2" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="J2" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="B3" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="C3" t="n">
-        <v>2005482</v>
+        <v>2005532</v>
       </c>
       <c r="D3" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="E3" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="F3" t="n">
         <v>75425</v>
       </c>
       <c r="G3" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="H3" t="n">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="I3" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="J3" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="B4" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="C4" t="n">
         <v>1138017</v>
       </c>
       <c r="D4" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="E4" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="F4" t="n">
-        <v>92612</v>
+        <v>92625</v>
       </c>
       <c r="G4" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="H4" t="n">
         <v>239</v>
@@ -2013,231 +2030,231 @@
         <v>322</v>
       </c>
       <c r="J4" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B5" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="C5" t="n">
-        <v>6982683</v>
+        <v>7259752</v>
       </c>
       <c r="D5" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="E5" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="F5" t="n">
         <v>25454</v>
       </c>
       <c r="G5" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="H5" t="n">
         <v>198</v>
       </c>
       <c r="I5" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="J5" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="B6" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="C6" t="n">
-        <v>7231111</v>
+        <v>6990662</v>
       </c>
       <c r="D6" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="E6" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="F6" t="n">
-        <v>134469</v>
+        <v>134525</v>
       </c>
       <c r="G6" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="H6" t="n">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="I6" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="J6" t="s">
-        <v>328</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="B7" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="C7" t="n">
         <v>4907461</v>
       </c>
       <c r="D7" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="E7" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="F7" t="n">
         <v>30413</v>
       </c>
       <c r="G7" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="H7" t="n">
         <v>162</v>
       </c>
       <c r="I7" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="J7" t="s">
-        <v>331</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="B8" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="C8" t="n">
         <v>1205516</v>
       </c>
       <c r="D8" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="E8" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="F8" t="n">
         <v>85290</v>
       </c>
       <c r="G8" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="H8" t="n">
         <v>146</v>
       </c>
       <c r="I8" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="J8" t="s">
-        <v>331</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="B9" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="C9" t="n">
-        <v>2893173</v>
+        <v>2893649</v>
       </c>
       <c r="D9" t="s">
         <v>322</v>
       </c>
       <c r="E9" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="F9" t="n">
-        <v>116095</v>
+        <v>116124</v>
       </c>
       <c r="G9" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="H9" t="n">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="I9" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="J9" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="B10" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="C10" t="n">
-        <v>4601749</v>
+        <v>4606413</v>
       </c>
       <c r="D10" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="E10" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="F10" t="n">
         <v>14703</v>
       </c>
       <c r="G10" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="H10" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I10" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="J10" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>326</v>
+      </c>
+      <c r="B11" t="s">
+        <v>268</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4087125</v>
+      </c>
+      <c r="D11" t="s">
+        <v>318</v>
+      </c>
+      <c r="E11" t="s">
+        <v>341</v>
+      </c>
+      <c r="F11" t="n">
+        <v>18451</v>
+      </c>
+      <c r="G11" t="s">
         <v>320</v>
       </c>
-      <c r="B11" t="s">
-        <v>262</v>
-      </c>
-      <c r="C11" t="n">
-        <v>4080180</v>
-      </c>
-      <c r="D11" t="s">
-        <v>312</v>
-      </c>
-      <c r="E11" t="s">
-        <v>336</v>
-      </c>
-      <c r="F11" t="n">
-        <v>18450</v>
-      </c>
-      <c r="G11" t="s">
-        <v>314</v>
-      </c>
       <c r="H11" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I11" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="J11" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2256,30 +2273,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
@@ -2287,41 +2304,41 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2340,25 +2357,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2">
@@ -2366,390 +2383,390 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>657692</v>
+        <v>618878</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F2" t="n">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="G2" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" t="n">
-        <v>52677</v>
+        <v>61813</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F3" t="n">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G3" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" t="n">
-        <v>72789</v>
+        <v>74336</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F4" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B5" t="n">
-        <v>33680</v>
+        <v>33379</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="F5" t="n">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="G5" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B6" t="n">
-        <v>23116</v>
+        <v>22305</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F6" t="n">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G6" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B7" t="n">
-        <v>5283</v>
+        <v>4443</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F7" t="n">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="G7" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B8" t="n">
-        <v>21406</v>
+        <v>18646</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F8" t="n">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="G8" t="n">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B9" t="n">
-        <v>52136</v>
+        <v>45289</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F9" t="n">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="G9" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B10" t="n">
-        <v>13495</v>
+        <v>12032</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F10" t="n">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="G10" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B11" t="n">
-        <v>77190</v>
+        <v>65050</v>
       </c>
       <c r="C11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" t="s">
         <v>75</v>
       </c>
-      <c r="D11" t="s">
-        <v>76</v>
-      </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="F11" t="n">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="G11" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B12" t="n">
-        <v>179372</v>
+        <v>166666</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F12" t="n">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="G12" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" t="n">
+        <v>29516</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" t="n">
         <v>80</v>
       </c>
-      <c r="B13" t="n">
-        <v>34327</v>
-      </c>
-      <c r="C13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" t="n">
-        <v>104</v>
-      </c>
       <c r="G13" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B14" t="n">
-        <v>8298</v>
+        <v>7327</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F14" t="n">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G14" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B15" t="n">
-        <v>22716</v>
+        <v>25395</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="F15" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G15" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B16" t="n">
-        <v>18944</v>
+        <v>18113</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F16" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="G16" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B17" t="n">
-        <v>29674</v>
+        <v>21025</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="E17" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="F17" t="n">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G17" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B18" t="n">
-        <v>12589</v>
+        <v>13543</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D18" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F18" t="n">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G18" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2768,200 +2785,200 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C7" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C10" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C11" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B15" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C16" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B17" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C17" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="C18" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19">
@@ -2969,10 +2986,21 @@
         <v>111</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="C19" t="s">
-        <v>135</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2991,86 +3019,86 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="D5" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="D6" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -3089,35 +3117,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -3128,83 +3156,83 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C4" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D4" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="D5" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="D6" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B7" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="D7" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B8" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C8" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B9" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C9" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D9" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3223,16 +3251,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
@@ -3240,97 +3268,97 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C2" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D2" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B3" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C3" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D3" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D4" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C5" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D5" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B6" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C6" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="D6" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B7" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C7" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="D7" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B8" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C8" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D8" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -3349,58 +3377,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B2" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C2" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D2" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B3" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C3" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="D3" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B4" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="C4" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3419,58 +3447,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B2" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="C2" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="D2" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B3" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="C3" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="D3" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B4" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C4" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="D4" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5">
@@ -3478,18 +3506,18 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="C5" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="D5" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="B6"/>
       <c r="C6"/>
@@ -3497,44 +3525,44 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B7" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="C7" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="D7" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B8" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C8" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="D8" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B9" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="C9" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="D9" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10">
@@ -3542,13 +3570,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="C10" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="D10" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>